<commit_message>
KIBON-288: Individuellen Zuschlag zum Erwerbspensum entfernen: Weitere Statistiken angepasst, Tets korrigiert
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchZeitraum.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchZeitraum.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\dev\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\G$\hefr\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{9861F8D9-0C2B-4FF4-967E-698DF2A77809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="2895" windowWidth="24465" windowHeight="13575"/>
+    <workbookView xWindow="-15" yWindow="2895" windowWidth="24465" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="5" r:id="rId1"/>
     <sheet name="Data" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DatapivotabelleData">Data!$A$1:$AB$2</definedName>
+    <definedName name="DatapivotabelleData">Data!$A$1:$AA$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <pivotCaches>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
   <si>
     <t>Institution</t>
   </si>
@@ -102,9 +103,6 @@
     <t>AnzahlVerfuegungenKeinPensum</t>
   </si>
   <si>
-    <t>AnzahlVerfuegungenZuschlagZumPensum</t>
-  </si>
-  <si>
     <t>AnzahlVerfuegungenNichtEintreten</t>
   </si>
   <si>
@@ -177,9 +175,6 @@
     <t>{anzahlVerfuegungenKeinPensum}</t>
   </si>
   <si>
-    <t>{anzahlVerfuegungenZuschlagZumPensum}</t>
-  </si>
-  <si>
     <t>{anzahlVerfuegungenNichtEintreten}</t>
   </si>
   <si>
@@ -261,9 +256,6 @@
     <t>Kein Pensum</t>
   </si>
   <si>
-    <t>Zuschlag zum Pensum</t>
-  </si>
-  <si>
     <t>Nichteintreten</t>
   </si>
   <si>
@@ -300,13 +292,13 @@
     <t>Ausgestellt</t>
   </si>
   <si>
-    <t>(All)</t>
+    <t>(Alle)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -422,17 +414,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -514,12 +495,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
@@ -552,20 +570,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -580,18 +598,907 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="236">
+  <dxfs count="354">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.249977111117893"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.249977111117893"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.249977111117893"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.249977111117893"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.249977111117893"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-0.249977111117893"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -2372,7 +3279,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42929.544201504628" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Herger Franziska" refreshedDate="43420.54963483796" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="DatapivotabelleData"/>
   </cacheSource>
@@ -2479,7 +3386,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
     <s v="{bgNummer}"/>
     <x v="0"/>
@@ -2514,8 +3421,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="B4:AB7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="B4:AA7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="30">
     <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -2555,7 +3462,7 @@
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -2575,7 +3482,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="25">
+  <colItems count="24">
     <i>
       <x/>
     </i>
@@ -2648,14 +3555,11 @@
     <i i="23">
       <x v="23"/>
     </i>
-    <i i="24">
-      <x v="24"/>
-    </i>
   </colItems>
   <pageFields count="1">
     <pageField fld="3" hier="-1"/>
   </pageFields>
-  <dataFields count="25">
+  <dataFields count="24">
     <dataField name="Total" fld="29" baseField="0" baseItem="0"/>
     <dataField name="Online" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Papier" fld="6" baseField="0" baseItem="0"/>
@@ -2679,11 +3583,10 @@
     <dataField name="Normale" fld="23" baseField="0" baseItem="0"/>
     <dataField name="Max Einkommen" fld="24" baseField="0" baseItem="0"/>
     <dataField name="Kein Pensum" fld="25" baseField="0" baseItem="0"/>
-    <dataField name="Zuschlag zum Pensum" fld="26" baseField="0" baseItem="0"/>
     <dataField name="Nichteintreten" fld="27" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="118">
-    <format dxfId="235">
+    <format dxfId="353">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -2694,7 +3597,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="234">
+    <format dxfId="352">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -2705,7 +3608,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="233">
+    <format dxfId="351">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -2716,7 +3619,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="232">
+    <format dxfId="350">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -2727,7 +3630,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="231">
+    <format dxfId="349">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -2747,7 +3650,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="230">
+    <format dxfId="348">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -2767,7 +3670,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="229">
+    <format dxfId="347">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2776,7 +3679,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="228">
+    <format dxfId="346">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2786,7 +3689,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="227">
+    <format dxfId="345">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -2797,7 +3700,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="226">
+    <format dxfId="344">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2806,7 +3709,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="225">
+    <format dxfId="343">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -2816,7 +3719,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="224">
+    <format dxfId="342">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -2827,7 +3730,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="223">
+    <format dxfId="341">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -2838,7 +3741,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="222">
+    <format dxfId="340">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -2849,7 +3752,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="221">
+    <format dxfId="339">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -2869,7 +3772,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="220">
+    <format dxfId="338">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -2889,26 +3792,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="219">
+    <format dxfId="337">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="218">
+    <format dxfId="336">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="217">
+    <format dxfId="335">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="216">
+    <format dxfId="334">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="215">
+    <format dxfId="333">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="214">
+    <format dxfId="332">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2916,10 +3819,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="213">
+    <format dxfId="331">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="23">
+          <reference field="4294967294" count="22">
             <x v="0"/>
             <x v="1"/>
             <x v="2"/>
@@ -2942,15 +3845,14 @@
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="212">
+    <format dxfId="330">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="23">
+          <reference field="4294967294" count="22">
             <x v="0"/>
             <x v="1"/>
             <x v="2"/>
@@ -2973,25 +3875,24 @@
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="211">
+    <format dxfId="329">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="210">
+    <format dxfId="328">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="209">
+    <format dxfId="327">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="208">
+    <format dxfId="326">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -2999,14 +3900,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="207">
+    <format dxfId="325">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="206">
+    <format dxfId="324">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3014,14 +3915,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="205">
+    <format dxfId="323">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="204">
+    <format dxfId="322">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3029,14 +3930,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="203">
+    <format dxfId="321">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="202">
+    <format dxfId="320">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3044,14 +3945,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="201">
+    <format dxfId="319">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="200">
+    <format dxfId="318">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3059,14 +3960,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="199">
+    <format dxfId="317">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="198">
+    <format dxfId="316">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3074,83 +3975,83 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="197">
+    <format dxfId="315">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="196">
+    <format dxfId="314">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="195">
+    <format dxfId="313">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="194">
+    <format dxfId="312">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="193">
+    <format dxfId="311">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="192">
+    <format dxfId="310">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="191">
+    <format dxfId="309">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="190">
+    <format dxfId="308">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="189">
+    <format dxfId="307">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="188">
+    <format dxfId="306">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="187">
+    <format dxfId="305">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="186">
+    <format dxfId="304">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="185">
+    <format dxfId="303">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3159,7 +4060,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="184">
+    <format dxfId="302">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3168,7 +4069,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="183">
+    <format dxfId="301">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -3179,13 +4080,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="182">
+    <format dxfId="300">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="181">
+    <format dxfId="299">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="A1:B1" fieldPosition="0"/>
     </format>
-    <format dxfId="180">
+    <format dxfId="298">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -3196,14 +4097,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="179">
+    <format dxfId="297">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="178">
+    <format dxfId="296">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3211,7 +4112,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="177">
+    <format dxfId="295">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -3231,7 +4132,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="176">
+    <format dxfId="294">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -3251,23 +4152,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="175">
+    <format dxfId="293">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="174">
+    <format dxfId="292">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="173">
+    <format dxfId="291">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="172">
+    <format dxfId="290">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="171">
+    <format dxfId="289">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3275,23 +4176,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="170">
+    <format dxfId="288">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="169">
+    <format dxfId="287">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="168">
+    <format dxfId="286">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="167">
+    <format dxfId="285">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="166">
+    <format dxfId="284">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3299,23 +4200,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="165">
+    <format dxfId="283">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="164">
+    <format dxfId="282">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="163">
+    <format dxfId="281">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="162">
+    <format dxfId="280">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="161">
+    <format dxfId="279">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3323,7 +4224,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="160">
+    <format dxfId="278">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -3334,13 +4235,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="159">
+    <format dxfId="277">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="158">
+    <format dxfId="276">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="A1:B1" fieldPosition="0"/>
     </format>
-    <format dxfId="157">
+    <format dxfId="275">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -3351,7 +4252,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="156">
+    <format dxfId="274">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -3371,10 +4272,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="155">
+    <format dxfId="273">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1:N1" fieldPosition="0"/>
     </format>
-    <format dxfId="154">
+    <format dxfId="272">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -3394,7 +4295,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="153">
+    <format dxfId="271">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -3403,10 +4304,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="152">
+    <format dxfId="270">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="O1" fieldPosition="0"/>
     </format>
-    <format dxfId="151">
+    <format dxfId="269">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3415,7 +4316,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="150">
+    <format dxfId="268">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -3424,10 +4325,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="149">
+    <format dxfId="267">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="R1" fieldPosition="0"/>
     </format>
-    <format dxfId="148">
+    <format dxfId="266">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3436,10 +4337,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="147">
+    <format dxfId="265">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="P1:Q1" fieldPosition="0"/>
     </format>
-    <format dxfId="146">
+    <format dxfId="264">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -3449,24 +4350,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="145">
+    <format dxfId="263">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
     </format>
-    <format dxfId="144">
+    <format dxfId="262">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="6">
+          <reference field="4294967294" count="5">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="143">
+    <format dxfId="261">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -3486,10 +4386,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="142">
+    <format dxfId="260">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1:N1" fieldPosition="0"/>
     </format>
-    <format dxfId="141">
+    <format dxfId="259">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -3509,23 +4409,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="140">
+    <format dxfId="258">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="139">
+    <format dxfId="257">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="138">
+    <format dxfId="256">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="137">
+    <format dxfId="255">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="136">
+    <format dxfId="254">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3533,7 +4433,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="135">
+    <format dxfId="253">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2" selected="0">
@@ -3543,10 +4443,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="134">
+    <format dxfId="252">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="P1:Q1" fieldPosition="0"/>
     </format>
-    <format dxfId="133">
+    <format dxfId="251">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -3556,69 +4456,65 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="132">
+    <format dxfId="250">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="6" selected="0">
+          <reference field="4294967294" count="5" selected="0">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="131">
+    <format dxfId="249">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
     </format>
-    <format dxfId="130">
+    <format dxfId="248">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="6">
+          <reference field="4294967294" count="5">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="129">
+    <format dxfId="247">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="6" selected="0">
+          <reference field="4294967294" count="5" selected="0">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="128">
+    <format dxfId="246">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
     </format>
-    <format dxfId="127">
+    <format dxfId="245">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="6">
+          <reference field="4294967294" count="5">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="126">
+    <format dxfId="244">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -3629,7 +4525,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="125">
+    <format dxfId="243">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -3640,7 +4536,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="124">
+    <format dxfId="242">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3649,7 +4545,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="123">
+    <format dxfId="241">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3658,7 +4554,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="122">
+    <format dxfId="240">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3667,51 +4563,48 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="121">
+    <format dxfId="239">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="6">
+          <reference field="4294967294" count="5">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="120">
+    <format dxfId="238">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="6">
+          <reference field="4294967294" count="5">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="119">
+    <format dxfId="237">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
-          <reference field="4294967294" count="6" selected="0">
+          <reference field="4294967294" count="5" selected="0">
             <x v="19"/>
             <x v="20"/>
             <x v="21"/>
             <x v="22"/>
             <x v="23"/>
-            <x v="24"/>
           </reference>
           <reference field="1" count="0" selected="0"/>
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="118">
+    <format dxfId="236">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -3729,7 +4622,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4024,17 +4917,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AB29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="S15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
@@ -4068,19 +4961,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="2:28" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
       <c r="G3" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
@@ -4094,29 +4987,29 @@
       <c r="Q3" s="25"/>
       <c r="R3" s="26"/>
       <c r="S3" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="T3" s="20" t="s">
-        <v>85</v>
+        <v>67</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="U3" s="22"/>
       <c r="V3" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="W3" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="22"/>
+        <v>69</v>
+      </c>
+      <c r="W3" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3"/>
     </row>
     <row r="4" spans="2:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -4141,7 +5034,6 @@
       <c r="Y4" s="19"/>
       <c r="Z4" s="19"/>
       <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
     </row>
     <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
@@ -4151,86 +5043,83 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="G5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="J5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="N5" s="14" t="s">
+      <c r="P5" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="Q5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="14" t="s">
-        <v>61</v>
-      </c>
       <c r="S5" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="U5" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="W5" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="X5" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="W5" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="X5" s="18" t="s">
+      <c r="Z5" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="AA5" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="Z5" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA5" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB5" s="18" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="27"/>
+        <v>25</v>
+      </c>
+      <c r="C6" s="20"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -4255,12 +5144,11 @@
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
       <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="11">
         <v>0</v>
@@ -4332,9 +5220,6 @@
         <v>0</v>
       </c>
       <c r="AA7" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4787,10 +5672,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="W3:AB3"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:R3"/>
     <mergeCell ref="T3:U3"/>
+    <mergeCell ref="W3:AA3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4798,14 +5683,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -4833,12 +5718,11 @@
     <col min="24" max="24" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4852,7 +5736,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -4897,10 +5781,10 @@
         <v>17</v>
       </c>
       <c r="T1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="U1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="V1" t="s">
         <v>18</v>
@@ -4920,97 +5804,91 @@
       <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" t="s">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>33</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>36</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>37</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>41</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U2" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" t="s">
         <v>42</v>
       </c>
-      <c r="T2" t="s">
-        <v>82</v>
-      </c>
-      <c r="U2" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>43</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>44</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>48</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
directToDev: pivot tables scroll fix / removed translation
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchZeitraum.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchZeitraum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\G$\hefr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egch\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{9861F8D9-0C2B-4FF4-967E-698DF2A77809}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB1AFD1-5A05-4C5F-B895-A88508011662}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="2895" windowWidth="24465" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="5" r:id="rId1"/>
@@ -537,9 +537,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -548,19 +547,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -573,7 +567,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -581,12 +575,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -599,6 +587,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -615,890 +609,7 @@
     <cellStyle name="20 % - Akzent1" xfId="1" builtinId="30"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="354">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-0.249977111117893"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thick">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="236">
     <dxf>
       <border>
         <left style="thin">
@@ -3279,11 +2390,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Herger Franziska" refreshedDate="43420.54963483796" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Egli Christian" refreshedDate="43531.499928472222" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="DatapivotabelleData"/>
   </cacheSource>
-  <cacheFields count="30">
+  <cacheFields count="29">
     <cacheField name="BGNummer" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -3368,9 +2479,6 @@
     <cacheField name="AnzahlVerfuegungenKeinPensum" numFmtId="0">
       <sharedItems/>
     </cacheField>
-    <cacheField name="AnzahlVerfuegungenZuschlagZumPensum" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
     <cacheField name="AnzahlVerfuegungenNichtEintreten" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -3414,7 +2522,6 @@
     <s v="{anzahlVerfuegungenNormal}"/>
     <s v="{anzahlVerfuegungenMaxEinkommen}"/>
     <s v="{anzahlVerfuegungenKeinPensum}"/>
-    <s v="{anzahlVerfuegungenZuschlagZumPensum}"/>
     <s v="{anzahlVerfuegungenNichtEintreten}"/>
   </r>
 </pivotCacheRecords>
@@ -3423,7 +2530,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" mergeItem="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B4:AA7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="30">
+  <pivotFields count="29">
     <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
       <items count="1">
@@ -3462,7 +2569,6 @@
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
@@ -3560,10 +2666,10 @@
     <pageField fld="3" hier="-1"/>
   </pageFields>
   <dataFields count="24">
-    <dataField name="Total" fld="29" baseField="0" baseItem="0"/>
+    <dataField name="Total" fld="28" baseField="0" baseItem="0"/>
     <dataField name="Online" fld="5" baseField="0" baseItem="0"/>
     <dataField name="Papier" fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Total " fld="28" baseField="1" baseItem="0"/>
+    <dataField name="Total " fld="27" baseField="1" baseItem="0"/>
     <dataField name="Online " fld="7" baseField="1" baseItem="0"/>
     <dataField name="Papier " fld="8" baseField="1" baseItem="0"/>
     <dataField name="Familien Situtation" fld="13" baseField="0" baseItem="0"/>
@@ -3583,10 +2689,10 @@
     <dataField name="Normale" fld="23" baseField="0" baseItem="0"/>
     <dataField name="Max Einkommen" fld="24" baseField="0" baseItem="0"/>
     <dataField name="Kein Pensum" fld="25" baseField="0" baseItem="0"/>
-    <dataField name="Nichteintreten" fld="27" baseField="0" baseItem="0"/>
+    <dataField name="Nichteintreten" fld="26" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="118">
-    <format dxfId="353">
+    <format dxfId="235">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -3597,7 +2703,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="352">
+    <format dxfId="234">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -3608,7 +2714,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="351">
+    <format dxfId="233">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -3619,7 +2725,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="350">
+    <format dxfId="232">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -3630,7 +2736,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="349">
+    <format dxfId="231">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -3650,7 +2756,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="348">
+    <format dxfId="230">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -3670,7 +2776,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="347">
+    <format dxfId="229">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3679,7 +2785,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="346">
+    <format dxfId="228">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -3689,7 +2795,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="345">
+    <format dxfId="227">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -3700,7 +2806,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="344">
+    <format dxfId="226">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -3709,7 +2815,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="343">
+    <format dxfId="225">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -3719,7 +2825,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="342">
+    <format dxfId="224">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -3730,7 +2836,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="341">
+    <format dxfId="223">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -3741,7 +2847,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="340">
+    <format dxfId="222">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -3752,7 +2858,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="339">
+    <format dxfId="221">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -3772,7 +2878,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="338">
+    <format dxfId="220">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -3792,26 +2898,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="337">
+    <format dxfId="219">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="336">
+    <format dxfId="218">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="335">
+    <format dxfId="217">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="334">
+    <format dxfId="216">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="333">
+    <format dxfId="215">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="332">
+    <format dxfId="214">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3819,7 +2925,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="331">
+    <format dxfId="213">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="22">
@@ -3849,7 +2955,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="330">
+    <format dxfId="212">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="22">
@@ -3879,20 +2985,20 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="329">
+    <format dxfId="211">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="328">
+    <format dxfId="210">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="327">
+    <format dxfId="209">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="326">
+    <format dxfId="208">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3900,14 +3006,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="325">
+    <format dxfId="207">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="324">
+    <format dxfId="206">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3915,14 +3021,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="323">
+    <format dxfId="205">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="322">
+    <format dxfId="204">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3930,14 +3036,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="321">
+    <format dxfId="203">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="320">
+    <format dxfId="202">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3945,14 +3051,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="319">
+    <format dxfId="201">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="318">
+    <format dxfId="200">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3960,14 +3066,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="317">
+    <format dxfId="199">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="316">
+    <format dxfId="198">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -3975,83 +3081,83 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="315">
+    <format dxfId="197">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="314">
+    <format dxfId="196">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="313">
+    <format dxfId="195">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="312">
+    <format dxfId="194">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="311">
+    <format dxfId="193">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="310">
+    <format dxfId="192">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="309">
+    <format dxfId="191">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="308">
+    <format dxfId="190">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="307">
+    <format dxfId="189">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="306">
+    <format dxfId="188">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="305">
+    <format dxfId="187">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="304">
+    <format dxfId="186">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="303">
+    <format dxfId="185">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4060,7 +3166,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="302">
+    <format dxfId="184">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4069,7 +3175,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="301">
+    <format dxfId="183">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -4080,13 +3186,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="300">
+    <format dxfId="182">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="299">
+    <format dxfId="181">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="A1:B1" fieldPosition="0"/>
     </format>
-    <format dxfId="298">
+    <format dxfId="180">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -4097,14 +3203,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="297">
+    <format dxfId="179">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="296">
+    <format dxfId="178">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -4112,7 +3218,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="295">
+    <format dxfId="177">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -4132,7 +3238,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="294">
+    <format dxfId="176">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -4152,23 +3258,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="293">
+    <format dxfId="175">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="292">
+    <format dxfId="174">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="291">
+    <format dxfId="173">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="290">
+    <format dxfId="172">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="289">
+    <format dxfId="171">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -4176,23 +3282,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="288">
+    <format dxfId="170">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="287">
+    <format dxfId="169">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="286">
+    <format dxfId="168">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="285">
+    <format dxfId="167">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="284">
+    <format dxfId="166">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -4200,23 +3306,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="283">
+    <format dxfId="165">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="282">
+    <format dxfId="164">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="281">
+    <format dxfId="163">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="280">
+    <format dxfId="162">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="279">
+    <format dxfId="161">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -4224,7 +3330,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="278">
+    <format dxfId="160">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3" selected="0">
@@ -4235,13 +3341,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="277">
+    <format dxfId="159">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="276">
+    <format dxfId="158">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="A1:B1" fieldPosition="0"/>
     </format>
-    <format dxfId="275">
+    <format dxfId="157">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -4252,7 +3358,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="274">
+    <format dxfId="156">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -4272,10 +3378,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="273">
+    <format dxfId="155">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1:N1" fieldPosition="0"/>
     </format>
-    <format dxfId="272">
+    <format dxfId="154">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -4295,7 +3401,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="271">
+    <format dxfId="153">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -4304,10 +3410,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="270">
+    <format dxfId="152">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="O1" fieldPosition="0"/>
     </format>
-    <format dxfId="269">
+    <format dxfId="151">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4316,7 +3422,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="268">
+    <format dxfId="150">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -4325,10 +3431,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="267">
+    <format dxfId="149">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="R1" fieldPosition="0"/>
     </format>
-    <format dxfId="266">
+    <format dxfId="148">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4337,10 +3443,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="265">
+    <format dxfId="147">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="P1:Q1" fieldPosition="0"/>
     </format>
-    <format dxfId="264">
+    <format dxfId="146">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -4350,10 +3456,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="263">
+    <format dxfId="145">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
     </format>
-    <format dxfId="262">
+    <format dxfId="144">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -4366,7 +3472,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="261">
+    <format dxfId="143">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12" selected="0">
@@ -4386,10 +3492,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="260">
+    <format dxfId="142">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="C1:N1" fieldPosition="0"/>
     </format>
-    <format dxfId="259">
+    <format dxfId="141">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="12">
@@ -4409,23 +3515,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="258">
+    <format dxfId="140">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="257">
+    <format dxfId="139">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="256">
+    <format dxfId="138">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="255">
+    <format dxfId="137">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="254">
+    <format dxfId="136">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -4433,7 +3539,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="253">
+    <format dxfId="135">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2" selected="0">
@@ -4443,10 +3549,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="252">
+    <format dxfId="134">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="P1:Q1" fieldPosition="0"/>
     </format>
-    <format dxfId="251">
+    <format dxfId="133">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -4456,7 +3562,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="250">
+    <format dxfId="132">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5" selected="0">
@@ -4469,10 +3575,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="249">
+    <format dxfId="131">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
     </format>
-    <format dxfId="248">
+    <format dxfId="130">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -4485,7 +3591,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="247">
+    <format dxfId="129">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5" selected="0">
@@ -4498,10 +3604,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="246">
+    <format dxfId="128">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" offset="S1:X1" fieldPosition="0"/>
     </format>
-    <format dxfId="245">
+    <format dxfId="127">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -4514,7 +3620,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="244">
+    <format dxfId="126">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -4525,7 +3631,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="243">
+    <format dxfId="125">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -4536,7 +3642,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="242">
+    <format dxfId="124">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4545,7 +3651,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="241">
+    <format dxfId="123">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4554,7 +3660,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="240">
+    <format dxfId="122">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4563,7 +3669,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="239">
+    <format dxfId="121">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -4576,7 +3682,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="238">
+    <format dxfId="120">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="5">
@@ -4589,7 +3695,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="237">
+    <format dxfId="119">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="5" selected="0">
@@ -4604,7 +3710,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="236">
+    <format dxfId="118">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" offset="IV256" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -4918,13 +4024,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AB29"/>
+  <dimension ref="B2:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="S15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="S6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Z22" sqref="Z22"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4956,719 +4062,274 @@
     <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="2:28" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="23" t="s">
+    <row r="3" spans="2:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="15" t="s">
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="11" t="s">
         <v>67</v>
       </c>
       <c r="T3" s="21" t="s">
         <v>82</v>
       </c>
       <c r="U3" s="22"/>
-      <c r="V3" s="16" t="s">
+      <c r="V3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="W3" s="27" t="s">
+      <c r="W3" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="25"/>
     </row>
-    <row r="4" spans="2:28" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="7" t="s">
+    <row r="4" spans="2:27" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
     </row>
-    <row r="5" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="14" t="s">
+      <c r="R5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="T5" s="14" t="s">
+      <c r="T5" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="U5" s="14" t="s">
+      <c r="U5" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="V5" s="4" t="s">
+      <c r="V5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="W5" s="18" t="s">
+      <c r="W5" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="X5" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="Y5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="Z5" s="18" t="s">
+      <c r="Z5" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="AA5" s="18" t="s">
+      <c r="AA5" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8" t="s">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>0</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>0</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="7">
         <v>0</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>0</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>0</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="7">
         <v>0</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <v>0</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="7">
         <v>0</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="7">
         <v>0</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="7">
         <v>0</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="7">
         <v>0</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="7">
         <v>0</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="7">
         <v>0</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="7">
         <v>0</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="8">
         <v>0</v>
       </c>
-      <c r="T7" s="10">
+      <c r="T7" s="7">
         <v>0</v>
       </c>
-      <c r="U7" s="10">
+      <c r="U7" s="7">
         <v>0</v>
       </c>
-      <c r="V7" s="11">
+      <c r="V7" s="8">
         <v>0</v>
       </c>
-      <c r="W7" s="17">
+      <c r="W7" s="13">
         <v>0</v>
       </c>
-      <c r="X7" s="17">
+      <c r="X7" s="13">
         <v>0</v>
       </c>
-      <c r="Y7" s="17">
+      <c r="Y7" s="13">
         <v>0</v>
       </c>
-      <c r="Z7" s="17">
+      <c r="Z7" s="13">
         <v>0</v>
       </c>
-      <c r="AA7" s="17">
+      <c r="AA7" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-    </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-    </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="AA13" s="5"/>
-    </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-      <c r="T25" s="6"/>
-      <c r="U25" s="6"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="AA13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5687,7 +4348,7 @@
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>